<commit_message>
fix: Update LR MASTER COPY template with cell height adjustments
- Adjust cell heights to ensure LR print fits on one page
- Optimize template layout for better printing
</commit_message>
<xml_diff>
--- a/LR MASTER COPY.xlsx
+++ b/LR MASTER COPY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LRBillingOnline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450BFD2F-2F16-46C1-A475-AE99DE9F6D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FB33A9-F9A1-42C3-B5A3-C21FBF14B87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="285" yWindow="0" windowWidth="28515" windowHeight="15600" xr2:uid="{DE475AD4-6C2B-44F0-BD6D-02953E55204C}"/>
   </bookViews>
@@ -649,6 +649,60 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -656,6 +710,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -674,69 +737,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1055,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F23933-DBB5-4C2B-AD8D-B2D1BB8DD30A}">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="Q49" sqref="Q49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,10 +1082,10 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="L1" s="62" t="s">
+      <c r="L1" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="62"/>
+      <c r="M1" s="69"/>
     </row>
     <row r="2" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -1095,8 +1095,8 @@
       <c r="F2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
@@ -1119,56 +1119,56 @@
       <c r="A4" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="73"/>
       <c r="K4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
     </row>
     <row r="5" spans="1:13" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A5" s="35"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="54"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="75"/>
       <c r="K5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
     </row>
     <row r="6" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="36"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="61"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="62"/>
       <c r="K6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="63"/>
-      <c r="M6" s="63"/>
-    </row>
-    <row r="7" spans="1:13" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+    </row>
+    <row r="7" spans="1:13" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -1187,56 +1187,56 @@
       <c r="A8" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="52"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="73"/>
       <c r="K8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="71"/>
     </row>
     <row r="9" spans="1:13" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A9" s="35"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="54"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="75"/>
       <c r="K9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="63"/>
-      <c r="M9" s="63"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
     </row>
     <row r="10" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="36"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="56"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="77"/>
       <c r="K10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="63"/>
-      <c r="M10" s="63"/>
-    </row>
-    <row r="11" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+    </row>
+    <row r="11" spans="1:13" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -1252,17 +1252,17 @@
       <c r="A12" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="75"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="54"/>
       <c r="K12" s="27" t="s">
         <v>15</v>
       </c>
@@ -1271,30 +1271,30 @@
     </row>
     <row r="13" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="40"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="59"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="65"/>
       <c r="K13" s="28"/>
       <c r="L13" s="22"/>
       <c r="M13" s="19"/>
     </row>
     <row r="14" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="50"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="68"/>
       <c r="K14" s="25" t="s">
         <v>16</v>
       </c>
@@ -1303,30 +1303,30 @@
     </row>
     <row r="15" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="41"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="50"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="68"/>
       <c r="K15" s="26"/>
       <c r="L15" s="22"/>
       <c r="M15" s="19"/>
     </row>
     <row r="16" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="50"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="68"/>
       <c r="K16" s="25" t="s">
         <v>17</v>
       </c>
@@ -1335,62 +1335,62 @@
     </row>
     <row r="17" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="41"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="50"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="68"/>
       <c r="K17" s="26"/>
       <c r="L17" s="22"/>
       <c r="M17" s="19"/>
     </row>
-    <row r="18" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="41"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="50"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="68"/>
       <c r="K18" s="25" t="s">
         <v>18</v>
       </c>
       <c r="L18" s="21"/>
-      <c r="M18" s="18"/>
+      <c r="M18" s="19"/>
     </row>
     <row r="19" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="41"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="50"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="68"/>
       <c r="K19" s="24"/>
       <c r="L19" s="22"/>
       <c r="M19" s="19"/>
     </row>
     <row r="20" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A20" s="41"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="50"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="68"/>
       <c r="K20" s="25" t="s">
         <v>20</v>
       </c>
@@ -1399,15 +1399,15 @@
     </row>
     <row r="21" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="41"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="50"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="68"/>
       <c r="K21" s="29"/>
       <c r="L21" s="22"/>
       <c r="M21" s="19"/>
@@ -1440,11 +1440,11 @@
       <c r="H23" s="46"/>
       <c r="I23" s="46"/>
       <c r="J23" s="47"/>
-      <c r="K23" s="66" t="s">
+      <c r="K23" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="L23" s="68"/>
-      <c r="M23" s="69"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="58"/>
     </row>
     <row r="24" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="23" t="s">
@@ -1459,9 +1459,9 @@
       <c r="H24" s="44"/>
       <c r="I24" s="44"/>
       <c r="J24" s="45"/>
-      <c r="K24" s="67"/>
-      <c r="L24" s="70"/>
-      <c r="M24" s="71"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="59"/>
+      <c r="M24" s="60"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G25" s="37" t="s">
@@ -1469,10 +1469,10 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L26" s="72" t="s">
+      <c r="L26" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="M26" s="72"/>
+      <c r="M26" s="50"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="38" t="s">
@@ -1486,10 +1486,10 @@
       <c r="M28" s="37"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L29" s="72" t="s">
+      <c r="L29" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="M29" s="72"/>
+      <c r="M29" s="50"/>
     </row>
     <row r="30" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A30" s="10" t="s">
@@ -1503,10 +1503,10 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-      <c r="L30" s="62" t="s">
+      <c r="L30" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="M30" s="62"/>
+      <c r="M30" s="69"/>
     </row>
     <row r="31" spans="1:13" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
@@ -1516,8 +1516,8 @@
       <c r="F31" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="L31" s="62"/>
-      <c r="M31" s="62"/>
+      <c r="L31" s="69"/>
+      <c r="M31" s="69"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
@@ -1540,66 +1540,66 @@
       <c r="A33" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="52"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="72"/>
+      <c r="F33" s="72"/>
+      <c r="G33" s="72"/>
+      <c r="H33" s="72"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="73"/>
       <c r="K33" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="L33" s="64"/>
-      <c r="M33" s="64"/>
+      <c r="L33" s="70"/>
+      <c r="M33" s="70"/>
     </row>
     <row r="34" spans="1:13" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A34" s="35"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
-      <c r="J34" s="54"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="75"/>
       <c r="K34" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="L34" s="63"/>
-      <c r="M34" s="63"/>
+      <c r="L34" s="51"/>
+      <c r="M34" s="51"/>
     </row>
     <row r="35" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="36"/>
-      <c r="B35" s="55"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="55"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="56"/>
+      <c r="B35" s="76"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="76"/>
+      <c r="F35" s="76"/>
+      <c r="G35" s="76"/>
+      <c r="H35" s="76"/>
+      <c r="I35" s="76"/>
+      <c r="J35" s="77"/>
       <c r="K35" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="L35" s="63"/>
-      <c r="M35" s="63"/>
-    </row>
-    <row r="36" spans="1:13" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L35" s="51"/>
+      <c r="M35" s="51"/>
+    </row>
+    <row r="36" spans="1:13" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="15"/>
-      <c r="B36" s="76"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="76"/>
-      <c r="G36" s="76"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="76"/>
-      <c r="J36" s="77"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="48"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="49"/>
       <c r="K36" s="11"/>
       <c r="L36" s="11"/>
       <c r="M36" s="16"/>
@@ -1608,56 +1608,56 @@
       <c r="A37" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="51"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="51"/>
-      <c r="I37" s="51"/>
-      <c r="J37" s="52"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="72"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="73"/>
       <c r="K37" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L37" s="65"/>
-      <c r="M37" s="65"/>
+      <c r="L37" s="71"/>
+      <c r="M37" s="71"/>
     </row>
     <row r="38" spans="1:13" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A38" s="35"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="53"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="54"/>
+      <c r="B38" s="74"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="75"/>
       <c r="K38" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L38" s="63"/>
-      <c r="M38" s="63"/>
+      <c r="L38" s="51"/>
+      <c r="M38" s="51"/>
     </row>
     <row r="39" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="36"/>
-      <c r="B39" s="60"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="60"/>
-      <c r="H39" s="60"/>
-      <c r="I39" s="60"/>
-      <c r="J39" s="61"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="61"/>
+      <c r="G39" s="61"/>
+      <c r="H39" s="61"/>
+      <c r="I39" s="61"/>
+      <c r="J39" s="62"/>
       <c r="K39" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L39" s="63"/>
-      <c r="M39" s="63"/>
-    </row>
-    <row r="40" spans="1:13" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L39" s="51"/>
+      <c r="M39" s="51"/>
+    </row>
+    <row r="40" spans="1:13" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
@@ -1673,17 +1673,17 @@
       <c r="A41" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B41" s="73" t="s">
+      <c r="B41" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="74"/>
-      <c r="D41" s="74"/>
-      <c r="E41" s="74"/>
-      <c r="F41" s="74"/>
-      <c r="G41" s="74"/>
-      <c r="H41" s="74"/>
-      <c r="I41" s="74"/>
-      <c r="J41" s="75"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="54"/>
       <c r="K41" s="27" t="s">
         <v>15</v>
       </c>
@@ -1692,30 +1692,30 @@
     </row>
     <row r="42" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="40"/>
-      <c r="B42" s="57"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58"/>
-      <c r="F42" s="58"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="58"/>
-      <c r="I42" s="58"/>
-      <c r="J42" s="59"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="64"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="64"/>
+      <c r="H42" s="64"/>
+      <c r="I42" s="64"/>
+      <c r="J42" s="65"/>
       <c r="K42" s="28"/>
       <c r="L42" s="22"/>
       <c r="M42" s="19"/>
     </row>
     <row r="43" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A43" s="41"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="49"/>
-      <c r="D43" s="49"/>
-      <c r="E43" s="49"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="50"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="67"/>
+      <c r="I43" s="67"/>
+      <c r="J43" s="68"/>
       <c r="K43" s="25" t="s">
         <v>16</v>
       </c>
@@ -1724,30 +1724,30 @@
     </row>
     <row r="44" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="41"/>
-      <c r="B44" s="48"/>
-      <c r="C44" s="49"/>
-      <c r="D44" s="49"/>
-      <c r="E44" s="49"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="49"/>
-      <c r="H44" s="49"/>
-      <c r="I44" s="49"/>
-      <c r="J44" s="50"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="67"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="67"/>
+      <c r="H44" s="67"/>
+      <c r="I44" s="67"/>
+      <c r="J44" s="68"/>
       <c r="K44" s="26"/>
       <c r="L44" s="22"/>
       <c r="M44" s="19"/>
     </row>
     <row r="45" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A45" s="41"/>
-      <c r="B45" s="48"/>
-      <c r="C45" s="49"/>
-      <c r="D45" s="49"/>
-      <c r="E45" s="49"/>
-      <c r="F45" s="49"/>
-      <c r="G45" s="49"/>
-      <c r="H45" s="49"/>
-      <c r="I45" s="49"/>
-      <c r="J45" s="50"/>
+      <c r="B45" s="66"/>
+      <c r="C45" s="67"/>
+      <c r="D45" s="67"/>
+      <c r="E45" s="67"/>
+      <c r="F45" s="67"/>
+      <c r="G45" s="67"/>
+      <c r="H45" s="67"/>
+      <c r="I45" s="67"/>
+      <c r="J45" s="68"/>
       <c r="K45" s="25" t="s">
         <v>17</v>
       </c>
@@ -1756,30 +1756,30 @@
     </row>
     <row r="46" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="41"/>
-      <c r="B46" s="48"/>
-      <c r="C46" s="49"/>
-      <c r="D46" s="49"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="49"/>
-      <c r="G46" s="49"/>
-      <c r="H46" s="49"/>
-      <c r="I46" s="49"/>
-      <c r="J46" s="50"/>
+      <c r="B46" s="66"/>
+      <c r="C46" s="67"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="67"/>
+      <c r="I46" s="67"/>
+      <c r="J46" s="68"/>
       <c r="K46" s="26"/>
       <c r="L46" s="22"/>
       <c r="M46" s="19"/>
     </row>
     <row r="47" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A47" s="41"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="49"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="49"/>
-      <c r="H47" s="49"/>
-      <c r="I47" s="49"/>
-      <c r="J47" s="50"/>
+      <c r="B47" s="66"/>
+      <c r="C47" s="67"/>
+      <c r="D47" s="67"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="67"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="67"/>
+      <c r="I47" s="67"/>
+      <c r="J47" s="68"/>
       <c r="K47" s="25" t="s">
         <v>18</v>
       </c>
@@ -1788,30 +1788,30 @@
     </row>
     <row r="48" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="41"/>
-      <c r="B48" s="48"/>
-      <c r="C48" s="49"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="49"/>
-      <c r="H48" s="49"/>
-      <c r="I48" s="49"/>
-      <c r="J48" s="50"/>
+      <c r="B48" s="66"/>
+      <c r="C48" s="67"/>
+      <c r="D48" s="67"/>
+      <c r="E48" s="67"/>
+      <c r="F48" s="67"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="67"/>
+      <c r="I48" s="67"/>
+      <c r="J48" s="68"/>
       <c r="K48" s="24"/>
       <c r="L48" s="22"/>
       <c r="M48" s="19"/>
     </row>
     <row r="49" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A49" s="41"/>
-      <c r="B49" s="48"/>
-      <c r="C49" s="49"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="49"/>
-      <c r="H49" s="49"/>
-      <c r="I49" s="49"/>
-      <c r="J49" s="50"/>
+      <c r="B49" s="66"/>
+      <c r="C49" s="67"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="67"/>
+      <c r="F49" s="67"/>
+      <c r="G49" s="67"/>
+      <c r="H49" s="67"/>
+      <c r="I49" s="67"/>
+      <c r="J49" s="68"/>
       <c r="K49" s="25" t="s">
         <v>20</v>
       </c>
@@ -1820,15 +1820,15 @@
     </row>
     <row r="50" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="41"/>
-      <c r="B50" s="48"/>
-      <c r="C50" s="49"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="49"/>
-      <c r="G50" s="49"/>
-      <c r="H50" s="49"/>
-      <c r="I50" s="49"/>
-      <c r="J50" s="50"/>
+      <c r="B50" s="66"/>
+      <c r="C50" s="67"/>
+      <c r="D50" s="67"/>
+      <c r="E50" s="67"/>
+      <c r="F50" s="67"/>
+      <c r="G50" s="67"/>
+      <c r="H50" s="67"/>
+      <c r="I50" s="67"/>
+      <c r="J50" s="68"/>
       <c r="K50" s="29"/>
       <c r="L50" s="22"/>
       <c r="M50" s="19"/>
@@ -1861,11 +1861,11 @@
       <c r="H52" s="46"/>
       <c r="I52" s="46"/>
       <c r="J52" s="47"/>
-      <c r="K52" s="66" t="s">
+      <c r="K52" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="L52" s="68"/>
-      <c r="M52" s="69"/>
+      <c r="L52" s="57"/>
+      <c r="M52" s="58"/>
     </row>
     <row r="53" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="39" t="s">
@@ -1880,9 +1880,9 @@
       <c r="H53" s="44"/>
       <c r="I53" s="44"/>
       <c r="J53" s="45"/>
-      <c r="K53" s="67"/>
-      <c r="L53" s="70"/>
-      <c r="M53" s="71"/>
+      <c r="K53" s="56"/>
+      <c r="L53" s="59"/>
+      <c r="M53" s="60"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G54" s="37" t="s">
@@ -1890,10 +1890,10 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L55" s="72" t="s">
+      <c r="L55" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="M55" s="72"/>
+      <c r="M55" s="50"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="38" t="s">
@@ -1907,13 +1907,51 @@
       <c r="M57" s="37"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L58" s="72" t="s">
+      <c r="L58" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="M58" s="72"/>
+      <c r="M58" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B50:J50"/>
+    <mergeCell ref="B33:J33"/>
+    <mergeCell ref="B34:J34"/>
+    <mergeCell ref="B35:J35"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="B38:J38"/>
+    <mergeCell ref="B10:J10"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="B9:J9"/>
+    <mergeCell ref="L1:M2"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="L23:M24"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B17:J17"/>
+    <mergeCell ref="B18:J18"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="L30:M31"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="L37:M37"/>
     <mergeCell ref="L55:M55"/>
     <mergeCell ref="L58:M58"/>
     <mergeCell ref="L38:M38"/>
@@ -1930,44 +1968,6 @@
     <mergeCell ref="B47:J47"/>
     <mergeCell ref="B48:J48"/>
     <mergeCell ref="B49:J49"/>
-    <mergeCell ref="L30:M31"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="L23:M24"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B17:J17"/>
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="L1:M2"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="B9:J9"/>
-    <mergeCell ref="B10:J10"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="B16:J16"/>
-    <mergeCell ref="B50:J50"/>
-    <mergeCell ref="B33:J33"/>
-    <mergeCell ref="B34:J34"/>
-    <mergeCell ref="B35:J35"/>
-    <mergeCell ref="B37:J37"/>
-    <mergeCell ref="B38:J38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>